<commit_message>
JNG-2359: Add ETL to create incremental rdbms model
</commit_message>
<xml_diff>
--- a/judo-tatami-rdbms2liquibase/src/test/resources/RdbmsIncrementalTests.xlsx
+++ b/judo-tatami-rdbms2liquibase/src/test/resources/RdbmsIncrementalTests.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\judo-ng\runtime\judo-tatami\judo-tatami-rdbms2liquibase\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260E662D-4F10-4E55-845C-39EC4E5B400F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83015BA9-3A20-436A-8695-67998D703341}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="495" windowWidth="23535" windowHeight="14790" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="23010" windowHeight="12930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CasesOriginal" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="915" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="950" uniqueCount="166">
   <si>
     <t>type</t>
   </si>
@@ -496,6 +496,33 @@
   </si>
   <si>
     <t>table8.id</t>
+  </si>
+  <si>
+    <t>table7.table6_1</t>
+  </si>
+  <si>
+    <t>table6_1</t>
+  </si>
+  <si>
+    <t>TABLE_6_1</t>
+  </si>
+  <si>
+    <t>table7.table5_1</t>
+  </si>
+  <si>
+    <t>table5_1</t>
+  </si>
+  <si>
+    <t>TABLE_5_1</t>
+  </si>
+  <si>
+    <t>VARCHAR</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>255</t>
   </si>
 </sst>
 </file>
@@ -1380,8 +1407,8 @@
   </sheetPr>
   <dimension ref="A1:K1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1441,10 +1468,10 @@
         <v>16</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I2" s="6" t="s">
         <v>18</v>
@@ -1476,10 +1503,10 @@
         <v>16</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I3" s="9" t="s">
         <v>18</v>
@@ -1511,10 +1538,10 @@
         <v>16</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I4" s="9" t="s">
         <v>18</v>
@@ -1546,10 +1573,10 @@
         <v>16</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I5" s="9" t="s">
         <v>18</v>
@@ -1581,10 +1608,10 @@
         <v>16</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I6" s="9" t="s">
         <v>18</v>
@@ -1616,10 +1643,10 @@
         <v>16</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I7" s="9" t="s">
         <v>18</v>
@@ -1651,10 +1678,10 @@
         <v>16</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I8" s="9" t="s">
         <v>18</v>
@@ -1686,10 +1713,10 @@
         <v>40</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I9" s="9" t="s">
         <v>18</v>
@@ -1721,10 +1748,10 @@
         <v>16</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I10" s="9" t="s">
         <v>18</v>
@@ -1756,10 +1783,10 @@
         <v>16</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I11" s="9" t="s">
         <v>18</v>
@@ -1791,10 +1818,10 @@
         <v>16</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I12" s="9" t="s">
         <v>18</v>
@@ -1826,10 +1853,10 @@
         <v>16</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="H13" s="9" t="s">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="I13" s="9" t="s">
         <v>18</v>
@@ -1934,7 +1961,7 @@
         <v>57</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I16" s="9" t="s">
         <v>18</v>
@@ -1969,7 +1996,7 @@
         <v>57</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I17" s="9" t="s">
         <v>18</v>
@@ -2001,10 +2028,10 @@
         <v>16</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H18" s="9" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I18" s="9" t="s">
         <v>18</v>
@@ -2036,10 +2063,10 @@
         <v>16</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="I19" s="9" t="s">
         <v>18</v>
@@ -2070,7 +2097,9 @@
       <c r="F20" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G20" s="19"/>
+      <c r="G20" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="H20" s="9" t="s">
         <v>18</v>
       </c>
@@ -2103,7 +2132,9 @@
       <c r="F21" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="19"/>
+      <c r="G21" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="H21" s="9" t="s">
         <v>18</v>
       </c>
@@ -2137,10 +2168,10 @@
         <v>16</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>53</v>
+        <v>163</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>18</v>
+        <v>165</v>
       </c>
       <c r="I22" s="9" t="s">
         <v>18</v>
@@ -2171,7 +2202,9 @@
       <c r="F23" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G23" s="19"/>
+      <c r="G23" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="H23" s="9" t="s">
         <v>18</v>
       </c>
@@ -2204,7 +2237,9 @@
       <c r="F24" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G24" s="19"/>
+      <c r="G24" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="H24" s="9" t="s">
         <v>18</v>
       </c>
@@ -2237,9 +2272,11 @@
       <c r="F25" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G25" s="19"/>
-      <c r="H25" s="9" t="s">
-        <v>18</v>
+      <c r="G25" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H25" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="I25" s="9" t="s">
         <v>18</v>
@@ -2270,9 +2307,11 @@
       <c r="F26" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="9" t="s">
-        <v>18</v>
+      <c r="G26" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H26" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="I26" s="9" t="s">
         <v>18</v>
@@ -2303,9 +2342,11 @@
       <c r="F27" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G27" s="19"/>
-      <c r="H27" s="9" t="s">
-        <v>18</v>
+      <c r="G27" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="I27" s="9" t="s">
         <v>18</v>
@@ -2336,11 +2377,11 @@
       <c r="F28" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G28" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H28" s="9" t="s">
-        <v>18</v>
+      <c r="G28" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H28" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="I28" s="9" t="s">
         <v>18</v>
@@ -2371,9 +2412,11 @@
       <c r="F29" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G29" s="19"/>
-      <c r="H29" s="9" t="s">
-        <v>18</v>
+      <c r="G29" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="I29" s="9" t="s">
         <v>18</v>
@@ -2404,7 +2447,9 @@
       <c r="F30" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G30" s="19"/>
+      <c r="G30" s="19" t="s">
+        <v>57</v>
+      </c>
       <c r="H30" s="9" t="s">
         <v>18</v>
       </c>
@@ -2437,11 +2482,11 @@
       <c r="F31" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G31" s="9" t="s">
+      <c r="G31" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H31" s="9" t="s">
-        <v>18</v>
+      <c r="H31" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="I31" s="9" t="s">
         <v>18</v>
@@ -2472,11 +2517,11 @@
       <c r="F32" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="9" t="s">
+      <c r="G32" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="H32" s="9" t="s">
-        <v>18</v>
+      <c r="H32" s="19" t="s">
+        <v>164</v>
       </c>
       <c r="I32" s="9" t="s">
         <v>18</v>
@@ -2546,7 +2591,7 @@
         <v>57</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I34" s="19" t="s">
         <v>18</v>
@@ -2581,7 +2626,7 @@
         <v>57</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I35" s="19" t="s">
         <v>18</v>
@@ -2616,7 +2661,7 @@
         <v>57</v>
       </c>
       <c r="H36" s="19" t="s">
-        <v>18</v>
+        <v>164</v>
       </c>
       <c r="I36" s="19" t="s">
         <v>18</v>
@@ -2629,30 +2674,74 @@
       </c>
     </row>
     <row r="37" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="8"/>
-      <c r="B37" s="9"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="9"/>
-      <c r="E37" s="9"/>
-      <c r="F37" s="9"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="9"/>
-      <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="10"/>
+      <c r="A37" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="D37" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="G37" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H37" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="38" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="8"/>
-      <c r="B38" s="9"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="9"/>
-      <c r="E38" s="9"/>
-      <c r="F38" s="9"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="9"/>
-      <c r="I38" s="9"/>
-      <c r="J38" s="9"/>
-      <c r="K38" s="10"/>
+      <c r="A38" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>158</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G38" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="H38" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="I38" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="39" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="8"/>
@@ -15178,8 +15267,8 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17046,8 +17135,8 @@
   </sheetPr>
   <dimension ref="A1:I1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G46" sqref="G46"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17764,25 +17853,33 @@
       </c>
     </row>
     <row r="47" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A47" s="51"/>
+      <c r="A47" s="51" t="s">
+        <v>160</v>
+      </c>
       <c r="B47" s="48"/>
       <c r="C47" s="48"/>
       <c r="D47" s="47"/>
       <c r="E47" s="47"/>
       <c r="F47" s="47"/>
       <c r="G47" s="47"/>
-      <c r="H47" s="47"/>
+      <c r="H47" s="47" t="s">
+        <v>143</v>
+      </c>
       <c r="I47" s="49"/>
     </row>
     <row r="48" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A48" s="51"/>
+      <c r="A48" s="51" t="s">
+        <v>157</v>
+      </c>
       <c r="B48" s="48"/>
       <c r="C48" s="48"/>
       <c r="D48" s="47"/>
       <c r="E48" s="47"/>
       <c r="F48" s="47"/>
       <c r="G48" s="47"/>
-      <c r="H48" s="47"/>
+      <c r="H48" s="47" t="s">
+        <v>143</v>
+      </c>
       <c r="I48" s="49"/>
     </row>
     <row r="49" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">

</xml_diff>